<commit_message>
data slipt 1 - 02
</commit_message>
<xml_diff>
--- a/data/data_split_1.xlsx
+++ b/data/data_split_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/khanh_nd204992_sis_hust_edu_vn/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D5B9C07-62BA-4D57-BAD2-7102048B914A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9832DF01-347B-45EB-8F53-307BFC53E84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9098,8 +9098,8 @@
   <dimension ref="A1:I2501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2268" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2276" sqref="F2276"/>
+      <pane ySplit="1" topLeftCell="A2496" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2502" sqref="E2502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -50058,6 +50058,9 @@
       <c r="D2277">
         <v>3</v>
       </c>
+      <c r="E2277">
+        <v>0</v>
+      </c>
     </row>
     <row r="2278" spans="1:7">
       <c r="A2278" s="1">
@@ -50072,6 +50075,9 @@
       <c r="D2278">
         <v>1</v>
       </c>
+      <c r="E2278">
+        <v>0</v>
+      </c>
     </row>
     <row r="2279" spans="1:7">
       <c r="A2279" s="1">
@@ -50086,6 +50092,9 @@
       <c r="D2279">
         <v>3</v>
       </c>
+      <c r="E2279">
+        <v>0</v>
+      </c>
     </row>
     <row r="2280" spans="1:7">
       <c r="A2280" s="1">
@@ -50100,6 +50109,9 @@
       <c r="D2280">
         <v>1</v>
       </c>
+      <c r="E2280">
+        <v>0</v>
+      </c>
     </row>
     <row r="2281" spans="1:7" ht="28.9">
       <c r="A2281" s="1">
@@ -50114,6 +50126,9 @@
       <c r="D2281">
         <v>1</v>
       </c>
+      <c r="F2281">
+        <v>0</v>
+      </c>
     </row>
     <row r="2282" spans="1:7" ht="28.9">
       <c r="A2282" s="1">
@@ -50128,6 +50143,9 @@
       <c r="D2282">
         <v>1</v>
       </c>
+      <c r="F2282">
+        <v>0</v>
+      </c>
     </row>
     <row r="2283" spans="1:7">
       <c r="A2283" s="1">
@@ -50142,6 +50160,9 @@
       <c r="D2283">
         <v>2</v>
       </c>
+      <c r="E2283">
+        <v>0</v>
+      </c>
     </row>
     <row r="2284" spans="1:7" ht="72">
       <c r="A2284" s="1">
@@ -50156,6 +50177,9 @@
       <c r="D2284">
         <v>2</v>
       </c>
+      <c r="E2284">
+        <v>0</v>
+      </c>
     </row>
     <row r="2285" spans="1:7" ht="57.6">
       <c r="A2285" s="1">
@@ -50170,6 +50194,9 @@
       <c r="D2285">
         <v>1</v>
       </c>
+      <c r="F2285">
+        <v>0</v>
+      </c>
     </row>
     <row r="2286" spans="1:7" ht="72">
       <c r="A2286" s="1">
@@ -50184,6 +50211,12 @@
       <c r="D2286">
         <v>2</v>
       </c>
+      <c r="E2286">
+        <v>0</v>
+      </c>
+      <c r="F2286">
+        <v>0</v>
+      </c>
     </row>
     <row r="2287" spans="1:7">
       <c r="A2287" s="1">
@@ -50198,6 +50231,9 @@
       <c r="D2287">
         <v>3</v>
       </c>
+      <c r="E2287">
+        <v>0</v>
+      </c>
     </row>
     <row r="2288" spans="1:7">
       <c r="A2288" s="1">
@@ -50212,8 +50248,14 @@
       <c r="D2288">
         <v>2</v>
       </c>
-    </row>
-    <row r="2289" spans="1:4">
+      <c r="F2288">
+        <v>0</v>
+      </c>
+      <c r="G2288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:8">
       <c r="A2289" s="1">
         <v>2287</v>
       </c>
@@ -50226,8 +50268,11 @@
       <c r="D2289">
         <v>3</v>
       </c>
-    </row>
-    <row r="2290" spans="1:4">
+      <c r="F2289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:8">
       <c r="A2290" s="1">
         <v>2288</v>
       </c>
@@ -50240,8 +50285,11 @@
       <c r="D2290">
         <v>3</v>
       </c>
-    </row>
-    <row r="2291" spans="1:4">
+      <c r="E2290">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:8">
       <c r="A2291" s="1">
         <v>2289</v>
       </c>
@@ -50254,8 +50302,11 @@
       <c r="D2291">
         <v>1</v>
       </c>
-    </row>
-    <row r="2292" spans="1:4">
+      <c r="E2291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:8">
       <c r="A2292" s="1">
         <v>2290</v>
       </c>
@@ -50268,8 +50319,11 @@
       <c r="D2292">
         <v>3</v>
       </c>
-    </row>
-    <row r="2293" spans="1:4">
+      <c r="E2292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:8">
       <c r="A2293" s="1">
         <v>2291</v>
       </c>
@@ -50282,8 +50336,11 @@
       <c r="D2293">
         <v>1</v>
       </c>
-    </row>
-    <row r="2294" spans="1:4" ht="43.15">
+      <c r="E2293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:8" ht="43.15">
       <c r="A2294" s="1">
         <v>2292</v>
       </c>
@@ -50296,8 +50353,17 @@
       <c r="D2294">
         <v>3</v>
       </c>
-    </row>
-    <row r="2295" spans="1:4" ht="28.9">
+      <c r="E2294">
+        <v>0</v>
+      </c>
+      <c r="F2294">
+        <v>-1</v>
+      </c>
+      <c r="H2294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:8" ht="28.9">
       <c r="A2295" s="1">
         <v>2293</v>
       </c>
@@ -50310,8 +50376,14 @@
       <c r="D2295">
         <v>2</v>
       </c>
-    </row>
-    <row r="2296" spans="1:4" ht="28.9">
+      <c r="E2295">
+        <v>0</v>
+      </c>
+      <c r="F2295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:8" ht="28.9">
       <c r="A2296" s="1">
         <v>2294</v>
       </c>
@@ -50324,8 +50396,11 @@
       <c r="D2296">
         <v>1</v>
       </c>
-    </row>
-    <row r="2297" spans="1:4" ht="43.15">
+      <c r="F2296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:8" ht="43.15">
       <c r="A2297" s="1">
         <v>2295</v>
       </c>
@@ -50338,8 +50413,11 @@
       <c r="D2297">
         <v>3</v>
       </c>
-    </row>
-    <row r="2298" spans="1:4" ht="28.9">
+      <c r="E2297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:8" ht="28.9">
       <c r="A2298" s="1">
         <v>2296</v>
       </c>
@@ -50352,8 +50430,11 @@
       <c r="D2298">
         <v>3</v>
       </c>
-    </row>
-    <row r="2299" spans="1:4">
+      <c r="H2298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:8">
       <c r="A2299" s="1">
         <v>2297</v>
       </c>
@@ -50366,8 +50447,11 @@
       <c r="D2299">
         <v>3</v>
       </c>
-    </row>
-    <row r="2300" spans="1:4">
+      <c r="E2299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:8">
       <c r="A2300" s="1">
         <v>2298</v>
       </c>
@@ -50380,8 +50464,11 @@
       <c r="D2300">
         <v>1</v>
       </c>
-    </row>
-    <row r="2301" spans="1:4">
+      <c r="E2300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:8">
       <c r="A2301" s="1">
         <v>2299</v>
       </c>
@@ -50394,8 +50481,11 @@
       <c r="D2301">
         <v>3</v>
       </c>
-    </row>
-    <row r="2302" spans="1:4">
+      <c r="E2301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:8">
       <c r="A2302" s="1">
         <v>2300</v>
       </c>
@@ -50408,8 +50498,11 @@
       <c r="D2302">
         <v>1</v>
       </c>
-    </row>
-    <row r="2303" spans="1:4" ht="43.15">
+      <c r="F2302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:8" ht="43.15">
       <c r="A2303" s="1">
         <v>2301</v>
       </c>
@@ -50422,8 +50515,11 @@
       <c r="D2303">
         <v>3</v>
       </c>
-    </row>
-    <row r="2304" spans="1:4">
+      <c r="F2303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:8">
       <c r="A2304" s="1">
         <v>2302</v>
       </c>
@@ -50436,8 +50532,14 @@
       <c r="D2304">
         <v>1</v>
       </c>
-    </row>
-    <row r="2305" spans="1:4">
+      <c r="E2304">
+        <v>0</v>
+      </c>
+      <c r="F2304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:8">
       <c r="A2305" s="1">
         <v>2303</v>
       </c>
@@ -50450,8 +50552,11 @@
       <c r="D2305">
         <v>1</v>
       </c>
-    </row>
-    <row r="2306" spans="1:4" ht="43.15">
+      <c r="E2305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:8" ht="43.15">
       <c r="A2306" s="1">
         <v>2304</v>
       </c>
@@ -50464,8 +50569,11 @@
       <c r="D2306">
         <v>1</v>
       </c>
-    </row>
-    <row r="2307" spans="1:4">
+      <c r="F2306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:8">
       <c r="A2307" s="1">
         <v>2305</v>
       </c>
@@ -50478,8 +50586,11 @@
       <c r="D2307">
         <v>1</v>
       </c>
-    </row>
-    <row r="2308" spans="1:4" ht="72">
+      <c r="E2307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:8" ht="72">
       <c r="A2308" s="1">
         <v>2306</v>
       </c>
@@ -50492,8 +50603,11 @@
       <c r="D2308">
         <v>1</v>
       </c>
-    </row>
-    <row r="2309" spans="1:4">
+      <c r="E2308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:8">
       <c r="A2309" s="1">
         <v>2307</v>
       </c>
@@ -50506,8 +50620,11 @@
       <c r="D2309">
         <v>1</v>
       </c>
-    </row>
-    <row r="2310" spans="1:4" ht="43.15">
+      <c r="E2309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:8" ht="43.15">
       <c r="A2310" s="1">
         <v>2308</v>
       </c>
@@ -50520,8 +50637,14 @@
       <c r="D2310">
         <v>1</v>
       </c>
-    </row>
-    <row r="2311" spans="1:4" ht="43.15">
+      <c r="E2310">
+        <v>0</v>
+      </c>
+      <c r="F2310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:8" ht="43.15">
       <c r="A2311" s="1">
         <v>2309</v>
       </c>
@@ -50534,8 +50657,11 @@
       <c r="D2311">
         <v>2</v>
       </c>
-    </row>
-    <row r="2312" spans="1:4" ht="28.9">
+      <c r="E2311">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:8" ht="28.9">
       <c r="A2312" s="1">
         <v>2310</v>
       </c>
@@ -50548,8 +50674,11 @@
       <c r="D2312">
         <v>2</v>
       </c>
-    </row>
-    <row r="2313" spans="1:4">
+      <c r="F2312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:8">
       <c r="A2313" s="1">
         <v>2311</v>
       </c>
@@ -50562,8 +50691,11 @@
       <c r="D2313">
         <v>2</v>
       </c>
-    </row>
-    <row r="2314" spans="1:4" ht="28.9">
+      <c r="E2313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:8" ht="28.9">
       <c r="A2314" s="1">
         <v>2312</v>
       </c>
@@ -50576,8 +50708,11 @@
       <c r="D2314">
         <v>3</v>
       </c>
-    </row>
-    <row r="2315" spans="1:4" ht="115.15">
+      <c r="E2314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:8" ht="115.15">
       <c r="A2315" s="1">
         <v>2313</v>
       </c>
@@ -50590,8 +50725,11 @@
       <c r="D2315">
         <v>1</v>
       </c>
-    </row>
-    <row r="2316" spans="1:4" ht="28.9">
+      <c r="E2315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:8" ht="28.9">
       <c r="A2316" s="1">
         <v>2314</v>
       </c>
@@ -50604,8 +50742,14 @@
       <c r="D2316">
         <v>1</v>
       </c>
-    </row>
-    <row r="2317" spans="1:4" ht="43.15">
+      <c r="E2316">
+        <v>0</v>
+      </c>
+      <c r="F2316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:8" ht="43.15">
       <c r="A2317" s="1">
         <v>2315</v>
       </c>
@@ -50618,8 +50762,14 @@
       <c r="D2317">
         <v>1</v>
       </c>
-    </row>
-    <row r="2318" spans="1:4" ht="28.9">
+      <c r="G2317">
+        <v>0</v>
+      </c>
+      <c r="H2317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:8" ht="28.9">
       <c r="A2318" s="1">
         <v>2316</v>
       </c>
@@ -50632,8 +50782,11 @@
       <c r="D2318">
         <v>1</v>
       </c>
-    </row>
-    <row r="2319" spans="1:4" ht="28.9">
+      <c r="E2318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:8" ht="28.9">
       <c r="A2319" s="1">
         <v>2317</v>
       </c>
@@ -50646,8 +50799,11 @@
       <c r="D2319">
         <v>1</v>
       </c>
-    </row>
-    <row r="2320" spans="1:4" ht="28.9">
+      <c r="E2319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:8" ht="28.9">
       <c r="A2320" s="1">
         <v>2318</v>
       </c>
@@ -50660,8 +50816,11 @@
       <c r="D2320">
         <v>3</v>
       </c>
-    </row>
-    <row r="2321" spans="1:4">
+      <c r="E2320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:8">
       <c r="A2321" s="1">
         <v>2319</v>
       </c>
@@ -50674,8 +50833,14 @@
       <c r="D2321">
         <v>1</v>
       </c>
-    </row>
-    <row r="2322" spans="1:4" ht="43.15">
+      <c r="E2321">
+        <v>0</v>
+      </c>
+      <c r="F2321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:8" ht="43.15">
       <c r="A2322" s="1">
         <v>2320</v>
       </c>
@@ -50688,8 +50853,11 @@
       <c r="D2322">
         <v>1</v>
       </c>
-    </row>
-    <row r="2323" spans="1:4">
+      <c r="F2322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:8">
       <c r="A2323" s="1">
         <v>2321</v>
       </c>
@@ -50702,8 +50870,14 @@
       <c r="D2323">
         <v>3</v>
       </c>
-    </row>
-    <row r="2324" spans="1:4">
+      <c r="E2323">
+        <v>1</v>
+      </c>
+      <c r="H2323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:8">
       <c r="A2324" s="1">
         <v>2322</v>
       </c>
@@ -50716,8 +50890,14 @@
       <c r="D2324">
         <v>1</v>
       </c>
-    </row>
-    <row r="2325" spans="1:4" ht="28.9">
+      <c r="F2324">
+        <v>0</v>
+      </c>
+      <c r="G2324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:8" ht="28.9">
       <c r="A2325" s="1">
         <v>2323</v>
       </c>
@@ -50730,8 +50910,11 @@
       <c r="D2325">
         <v>3</v>
       </c>
-    </row>
-    <row r="2326" spans="1:4">
+      <c r="E2325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:8">
       <c r="A2326" s="1">
         <v>2324</v>
       </c>
@@ -50744,8 +50927,11 @@
       <c r="D2326">
         <v>1</v>
       </c>
-    </row>
-    <row r="2327" spans="1:4">
+      <c r="E2326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:8">
       <c r="A2327" s="1">
         <v>2325</v>
       </c>
@@ -50758,8 +50944,11 @@
       <c r="D2327">
         <v>1</v>
       </c>
-    </row>
-    <row r="2328" spans="1:4">
+      <c r="H2327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:8">
       <c r="A2328" s="1">
         <v>2326</v>
       </c>
@@ -50772,8 +50961,14 @@
       <c r="D2328">
         <v>1</v>
       </c>
-    </row>
-    <row r="2329" spans="1:4" ht="28.9">
+      <c r="F2328">
+        <v>-1</v>
+      </c>
+      <c r="G2328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:8" ht="28.9">
       <c r="A2329" s="1">
         <v>2327</v>
       </c>
@@ -50786,8 +50981,14 @@
       <c r="D2329">
         <v>2</v>
       </c>
-    </row>
-    <row r="2330" spans="1:4" ht="28.9">
+      <c r="E2329">
+        <v>0</v>
+      </c>
+      <c r="H2329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:8" ht="28.9">
       <c r="A2330" s="1">
         <v>2328</v>
       </c>
@@ -50800,8 +51001,11 @@
       <c r="D2330">
         <v>2</v>
       </c>
-    </row>
-    <row r="2331" spans="1:4">
+      <c r="G2330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:8">
       <c r="A2331" s="1">
         <v>2329</v>
       </c>
@@ -50814,8 +51018,14 @@
       <c r="D2331">
         <v>3</v>
       </c>
-    </row>
-    <row r="2332" spans="1:4">
+      <c r="E2331">
+        <v>0</v>
+      </c>
+      <c r="H2331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:8">
       <c r="A2332" s="1">
         <v>2330</v>
       </c>
@@ -50828,8 +51038,11 @@
       <c r="D2332">
         <v>3</v>
       </c>
-    </row>
-    <row r="2333" spans="1:4" ht="86.45">
+      <c r="G2332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:8" ht="86.45">
       <c r="A2333" s="1">
         <v>2331</v>
       </c>
@@ -50842,8 +51055,11 @@
       <c r="D2333">
         <v>3</v>
       </c>
-    </row>
-    <row r="2334" spans="1:4" ht="28.9">
+      <c r="F2333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:8" ht="28.9">
       <c r="A2334" s="1">
         <v>2332</v>
       </c>
@@ -50856,8 +51072,11 @@
       <c r="D2334">
         <v>1</v>
       </c>
-    </row>
-    <row r="2335" spans="1:4" ht="28.9">
+      <c r="F2334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:8" ht="28.9">
       <c r="A2335" s="1">
         <v>2333</v>
       </c>
@@ -50870,8 +51089,14 @@
       <c r="D2335">
         <v>1</v>
       </c>
-    </row>
-    <row r="2336" spans="1:4">
+      <c r="G2335">
+        <v>0</v>
+      </c>
+      <c r="H2335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:8">
       <c r="A2336" s="1">
         <v>2334</v>
       </c>
@@ -50884,8 +51109,11 @@
       <c r="D2336">
         <v>3</v>
       </c>
-    </row>
-    <row r="2337" spans="1:4">
+      <c r="E2336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:8">
       <c r="A2337" s="1">
         <v>2335</v>
       </c>
@@ -50898,8 +51126,11 @@
       <c r="D2337">
         <v>1</v>
       </c>
-    </row>
-    <row r="2338" spans="1:4">
+      <c r="E2337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:8">
       <c r="A2338" s="1">
         <v>2336</v>
       </c>
@@ -50912,8 +51143,11 @@
       <c r="D2338">
         <v>1</v>
       </c>
-    </row>
-    <row r="2339" spans="1:4" ht="43.15">
+      <c r="E2338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:8" ht="43.15">
       <c r="A2339" s="1">
         <v>2337</v>
       </c>
@@ -50926,8 +51160,14 @@
       <c r="D2339">
         <v>2</v>
       </c>
-    </row>
-    <row r="2340" spans="1:4">
+      <c r="E2339">
+        <v>0</v>
+      </c>
+      <c r="F2339">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:8">
       <c r="A2340" s="1">
         <v>2338</v>
       </c>
@@ -50940,8 +51180,11 @@
       <c r="D2340">
         <v>1</v>
       </c>
-    </row>
-    <row r="2341" spans="1:4">
+      <c r="F2340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:8">
       <c r="A2341" s="1">
         <v>2339</v>
       </c>
@@ -50954,8 +51197,17 @@
       <c r="D2341">
         <v>1</v>
       </c>
-    </row>
-    <row r="2342" spans="1:4">
+      <c r="E2341">
+        <v>0</v>
+      </c>
+      <c r="G2341">
+        <v>1</v>
+      </c>
+      <c r="H2341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:8">
       <c r="A2342" s="1">
         <v>2340</v>
       </c>
@@ -50968,8 +51220,11 @@
       <c r="D2342">
         <v>1</v>
       </c>
-    </row>
-    <row r="2343" spans="1:4">
+      <c r="F2342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:8">
       <c r="A2343" s="1">
         <v>2341</v>
       </c>
@@ -50982,8 +51237,11 @@
       <c r="D2343">
         <v>2</v>
       </c>
-    </row>
-    <row r="2344" spans="1:4" ht="28.9">
+      <c r="F2343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:8" ht="28.9">
       <c r="A2344" s="1">
         <v>2342</v>
       </c>
@@ -50996,8 +51254,11 @@
       <c r="D2344">
         <v>3</v>
       </c>
-    </row>
-    <row r="2345" spans="1:4">
+      <c r="E2344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:8">
       <c r="A2345" s="1">
         <v>2343</v>
       </c>
@@ -51010,8 +51271,11 @@
       <c r="D2345">
         <v>3</v>
       </c>
-    </row>
-    <row r="2346" spans="1:4" ht="43.15">
+      <c r="E2345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:8" ht="43.15">
       <c r="A2346" s="1">
         <v>2344</v>
       </c>
@@ -51024,8 +51288,11 @@
       <c r="D2346">
         <v>1</v>
       </c>
-    </row>
-    <row r="2347" spans="1:4" ht="28.9">
+      <c r="H2346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:8" ht="28.9">
       <c r="A2347" s="1">
         <v>2345</v>
       </c>
@@ -51038,8 +51305,11 @@
       <c r="D2347">
         <v>2</v>
       </c>
-    </row>
-    <row r="2348" spans="1:4">
+      <c r="E2347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:8">
       <c r="A2348" s="1">
         <v>2346</v>
       </c>
@@ -51052,8 +51322,11 @@
       <c r="D2348">
         <v>1</v>
       </c>
-    </row>
-    <row r="2349" spans="1:4">
+      <c r="E2348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:8">
       <c r="A2349" s="1">
         <v>2347</v>
       </c>
@@ -51066,8 +51339,11 @@
       <c r="D2349">
         <v>2</v>
       </c>
-    </row>
-    <row r="2350" spans="1:4" ht="43.15">
+      <c r="E2349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:8" ht="43.15">
       <c r="A2350" s="1">
         <v>2348</v>
       </c>
@@ -51080,8 +51356,14 @@
       <c r="D2350">
         <v>1</v>
       </c>
-    </row>
-    <row r="2351" spans="1:4">
+      <c r="E2350">
+        <v>0</v>
+      </c>
+      <c r="F2350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:8">
       <c r="A2351" s="1">
         <v>2349</v>
       </c>
@@ -51094,8 +51376,11 @@
       <c r="D2351">
         <v>1</v>
       </c>
-    </row>
-    <row r="2352" spans="1:4" ht="28.9">
+      <c r="E2351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:8" ht="28.9">
       <c r="A2352" s="1">
         <v>2350</v>
       </c>
@@ -51108,8 +51393,11 @@
       <c r="D2352">
         <v>1</v>
       </c>
-    </row>
-    <row r="2353" spans="1:4" ht="43.15">
+      <c r="F2352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:8" ht="43.15">
       <c r="A2353" s="1">
         <v>2351</v>
       </c>
@@ -51122,8 +51410,14 @@
       <c r="D2353">
         <v>2</v>
       </c>
-    </row>
-    <row r="2354" spans="1:4" ht="28.9">
+      <c r="E2353">
+        <v>0</v>
+      </c>
+      <c r="F2353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:8" ht="28.9">
       <c r="A2354" s="1">
         <v>2352</v>
       </c>
@@ -51136,8 +51430,11 @@
       <c r="D2354">
         <v>2</v>
       </c>
-    </row>
-    <row r="2355" spans="1:4">
+      <c r="H2354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:8">
       <c r="A2355" s="1">
         <v>2353</v>
       </c>
@@ -51150,8 +51447,11 @@
       <c r="D2355">
         <v>3</v>
       </c>
-    </row>
-    <row r="2356" spans="1:4" ht="28.9">
+      <c r="E2355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:8" ht="28.9">
       <c r="A2356" s="1">
         <v>2354</v>
       </c>
@@ -51164,8 +51464,11 @@
       <c r="D2356">
         <v>3</v>
       </c>
-    </row>
-    <row r="2357" spans="1:4" ht="28.9">
+      <c r="H2356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:8" ht="28.9">
       <c r="A2357" s="1">
         <v>2355</v>
       </c>
@@ -51178,8 +51481,14 @@
       <c r="D2357">
         <v>3</v>
       </c>
-    </row>
-    <row r="2358" spans="1:4" ht="187.15">
+      <c r="E2357">
+        <v>1</v>
+      </c>
+      <c r="F2357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:8" ht="187.15">
       <c r="A2358" s="1">
         <v>2356</v>
       </c>
@@ -51192,8 +51501,11 @@
       <c r="D2358">
         <v>1</v>
       </c>
-    </row>
-    <row r="2359" spans="1:4">
+      <c r="F2358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:8">
       <c r="A2359" s="1">
         <v>2357</v>
       </c>
@@ -51206,8 +51518,11 @@
       <c r="D2359">
         <v>3</v>
       </c>
-    </row>
-    <row r="2360" spans="1:4" ht="43.15">
+      <c r="E2359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:8" ht="43.15">
       <c r="A2360" s="1">
         <v>2358</v>
       </c>
@@ -51220,8 +51535,11 @@
       <c r="D2360">
         <v>1</v>
       </c>
-    </row>
-    <row r="2361" spans="1:4">
+      <c r="F2360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:8">
       <c r="A2361" s="1">
         <v>2359</v>
       </c>
@@ -51234,8 +51552,11 @@
       <c r="D2361">
         <v>1</v>
       </c>
-    </row>
-    <row r="2362" spans="1:4" ht="43.15">
+      <c r="E2361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:8" ht="43.15">
       <c r="A2362" s="1">
         <v>2360</v>
       </c>
@@ -51248,8 +51569,17 @@
       <c r="D2362">
         <v>2</v>
       </c>
-    </row>
-    <row r="2363" spans="1:4">
+      <c r="E2362">
+        <v>1</v>
+      </c>
+      <c r="F2362">
+        <v>0</v>
+      </c>
+      <c r="G2362">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:8">
       <c r="A2363" s="1">
         <v>2361</v>
       </c>
@@ -51262,8 +51592,11 @@
       <c r="D2363">
         <v>3</v>
       </c>
-    </row>
-    <row r="2364" spans="1:4">
+      <c r="E2363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:8">
       <c r="A2364" s="1">
         <v>2362</v>
       </c>
@@ -51276,8 +51609,11 @@
       <c r="D2364">
         <v>1</v>
       </c>
-    </row>
-    <row r="2365" spans="1:4">
+      <c r="E2364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:8">
       <c r="A2365" s="1">
         <v>2363</v>
       </c>
@@ -51290,8 +51626,11 @@
       <c r="D2365">
         <v>2</v>
       </c>
-    </row>
-    <row r="2366" spans="1:4">
+      <c r="E2365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:8">
       <c r="A2366" s="1">
         <v>2364</v>
       </c>
@@ -51304,8 +51643,11 @@
       <c r="D2366">
         <v>3</v>
       </c>
-    </row>
-    <row r="2367" spans="1:4">
+      <c r="E2366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:8">
       <c r="A2367" s="1">
         <v>2365</v>
       </c>
@@ -51318,8 +51660,11 @@
       <c r="D2367">
         <v>1</v>
       </c>
-    </row>
-    <row r="2368" spans="1:4">
+      <c r="E2367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:8">
       <c r="A2368" s="1">
         <v>2366</v>
       </c>
@@ -51332,8 +51677,11 @@
       <c r="D2368">
         <v>3</v>
       </c>
-    </row>
-    <row r="2369" spans="1:4">
+      <c r="E2368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:8">
       <c r="A2369" s="1">
         <v>2367</v>
       </c>
@@ -51346,8 +51694,11 @@
       <c r="D2369">
         <v>3</v>
       </c>
-    </row>
-    <row r="2370" spans="1:4" ht="28.9">
+      <c r="E2369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:8" ht="28.9">
       <c r="A2370" s="1">
         <v>2368</v>
       </c>
@@ -51360,8 +51711,11 @@
       <c r="D2370">
         <v>2</v>
       </c>
-    </row>
-    <row r="2371" spans="1:4" ht="57.6">
+      <c r="E2370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:8" ht="57.6">
       <c r="A2371" s="1">
         <v>2369</v>
       </c>
@@ -51374,8 +51728,14 @@
       <c r="D2371">
         <v>1</v>
       </c>
-    </row>
-    <row r="2372" spans="1:4">
+      <c r="E2371">
+        <v>0</v>
+      </c>
+      <c r="F2371">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:8">
       <c r="A2372" s="1">
         <v>2370</v>
       </c>
@@ -51388,8 +51748,11 @@
       <c r="D2372">
         <v>3</v>
       </c>
-    </row>
-    <row r="2373" spans="1:4" ht="43.15">
+      <c r="E2372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:8" ht="43.15">
       <c r="A2373" s="1">
         <v>2371</v>
       </c>
@@ -51402,8 +51765,14 @@
       <c r="D2373">
         <v>3</v>
       </c>
-    </row>
-    <row r="2374" spans="1:4" ht="72">
+      <c r="E2373">
+        <v>0</v>
+      </c>
+      <c r="F2373">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:8" ht="72">
       <c r="A2374" s="1">
         <v>2372</v>
       </c>
@@ -51416,8 +51785,11 @@
       <c r="D2374">
         <v>1</v>
       </c>
-    </row>
-    <row r="2375" spans="1:4" ht="72">
+      <c r="E2374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:8" ht="72">
       <c r="A2375" s="1">
         <v>2373</v>
       </c>
@@ -51430,8 +51802,11 @@
       <c r="D2375">
         <v>2</v>
       </c>
-    </row>
-    <row r="2376" spans="1:4">
+      <c r="E2375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:8">
       <c r="A2376" s="1">
         <v>2374</v>
       </c>
@@ -51444,8 +51819,11 @@
       <c r="D2376">
         <v>3</v>
       </c>
-    </row>
-    <row r="2377" spans="1:4">
+      <c r="E2376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:8">
       <c r="A2377" s="1">
         <v>2375</v>
       </c>
@@ -51458,8 +51836,11 @@
       <c r="D2377">
         <v>3</v>
       </c>
-    </row>
-    <row r="2378" spans="1:4" ht="28.9">
+      <c r="E2377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:8" ht="28.9">
       <c r="A2378" s="1">
         <v>2376</v>
       </c>
@@ -51472,8 +51853,17 @@
       <c r="D2378">
         <v>1</v>
       </c>
-    </row>
-    <row r="2379" spans="1:4">
+      <c r="E2378">
+        <v>0</v>
+      </c>
+      <c r="G2378">
+        <v>1</v>
+      </c>
+      <c r="H2378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:8">
       <c r="A2379" s="1">
         <v>2377</v>
       </c>
@@ -51486,8 +51876,11 @@
       <c r="D2379">
         <v>1</v>
       </c>
-    </row>
-    <row r="2380" spans="1:4" ht="28.9">
+      <c r="E2379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:8" ht="28.9">
       <c r="A2380" s="1">
         <v>2378</v>
       </c>
@@ -51500,8 +51893,14 @@
       <c r="D2380">
         <v>2</v>
       </c>
-    </row>
-    <row r="2381" spans="1:4">
+      <c r="E2380">
+        <v>1</v>
+      </c>
+      <c r="H2380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:8">
       <c r="A2381" s="1">
         <v>2379</v>
       </c>
@@ -51514,8 +51913,11 @@
       <c r="D2381">
         <v>3</v>
       </c>
-    </row>
-    <row r="2382" spans="1:4">
+      <c r="E2381">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:8">
       <c r="A2382" s="1">
         <v>2380</v>
       </c>
@@ -51528,8 +51930,11 @@
       <c r="D2382">
         <v>1</v>
       </c>
-    </row>
-    <row r="2383" spans="1:4" ht="43.15">
+      <c r="G2382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:8" ht="43.15">
       <c r="A2383" s="1">
         <v>2381</v>
       </c>
@@ -51542,8 +51947,14 @@
       <c r="D2383">
         <v>3</v>
       </c>
-    </row>
-    <row r="2384" spans="1:4">
+      <c r="F2383">
+        <v>1</v>
+      </c>
+      <c r="H2383">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:8">
       <c r="A2384" s="1">
         <v>2382</v>
       </c>
@@ -51556,8 +51967,11 @@
       <c r="D2384">
         <v>3</v>
       </c>
-    </row>
-    <row r="2385" spans="1:4">
+      <c r="E2384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:8">
       <c r="A2385" s="1">
         <v>2383</v>
       </c>
@@ -51570,8 +51984,11 @@
       <c r="D2385">
         <v>1</v>
       </c>
-    </row>
-    <row r="2386" spans="1:4" ht="43.15">
+      <c r="E2385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:8" ht="43.15">
       <c r="A2386" s="1">
         <v>2384</v>
       </c>
@@ -51584,8 +52001,17 @@
       <c r="D2386">
         <v>3</v>
       </c>
-    </row>
-    <row r="2387" spans="1:4" ht="28.9">
+      <c r="E2386">
+        <v>1</v>
+      </c>
+      <c r="G2386">
+        <v>0</v>
+      </c>
+      <c r="H2386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:8" ht="28.9">
       <c r="A2387" s="1">
         <v>2385</v>
       </c>
@@ -51598,8 +52024,11 @@
       <c r="D2387">
         <v>1</v>
       </c>
-    </row>
-    <row r="2388" spans="1:4" ht="28.9">
+      <c r="H2387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:8" ht="28.9">
       <c r="A2388" s="1">
         <v>2386</v>
       </c>
@@ -51612,8 +52041,11 @@
       <c r="D2388">
         <v>1</v>
       </c>
-    </row>
-    <row r="2389" spans="1:4">
+      <c r="G2388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:8">
       <c r="A2389" s="1">
         <v>2387</v>
       </c>
@@ -51626,8 +52058,11 @@
       <c r="D2389">
         <v>1</v>
       </c>
-    </row>
-    <row r="2390" spans="1:4" ht="57.6">
+      <c r="E2389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:8" ht="57.6">
       <c r="A2390" s="1">
         <v>2388</v>
       </c>
@@ -51640,8 +52075,14 @@
       <c r="D2390">
         <v>1</v>
       </c>
-    </row>
-    <row r="2391" spans="1:4" ht="57.6">
+      <c r="E2390">
+        <v>0</v>
+      </c>
+      <c r="G2390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:8" ht="57.6">
       <c r="A2391" s="1">
         <v>2389</v>
       </c>
@@ -51654,8 +52095,14 @@
       <c r="D2391">
         <v>1</v>
       </c>
-    </row>
-    <row r="2392" spans="1:4">
+      <c r="E2391">
+        <v>0</v>
+      </c>
+      <c r="G2391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:8">
       <c r="A2392" s="1">
         <v>2390</v>
       </c>
@@ -51668,8 +52115,11 @@
       <c r="D2392">
         <v>1</v>
       </c>
-    </row>
-    <row r="2393" spans="1:4">
+      <c r="E2392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:8">
       <c r="A2393" s="1">
         <v>2391</v>
       </c>
@@ -51682,8 +52132,11 @@
       <c r="D2393">
         <v>3</v>
       </c>
-    </row>
-    <row r="2394" spans="1:4">
+      <c r="E2393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:8">
       <c r="A2394" s="1">
         <v>2392</v>
       </c>
@@ -51696,8 +52149,11 @@
       <c r="D2394">
         <v>2</v>
       </c>
-    </row>
-    <row r="2395" spans="1:4" ht="28.9">
+      <c r="E2394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:8" ht="28.9">
       <c r="A2395" s="1">
         <v>2393</v>
       </c>
@@ -51710,8 +52166,11 @@
       <c r="D2395">
         <v>3</v>
       </c>
-    </row>
-    <row r="2396" spans="1:4">
+      <c r="E2395">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:8">
       <c r="A2396" s="1">
         <v>2394</v>
       </c>
@@ -51724,8 +52183,11 @@
       <c r="D2396">
         <v>3</v>
       </c>
-    </row>
-    <row r="2397" spans="1:4">
+      <c r="E2396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:8">
       <c r="A2397" s="1">
         <v>2395</v>
       </c>
@@ -51738,8 +52200,11 @@
       <c r="D2397">
         <v>2</v>
       </c>
-    </row>
-    <row r="2398" spans="1:4">
+      <c r="E2397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:8">
       <c r="A2398" s="1">
         <v>2396</v>
       </c>
@@ -51752,8 +52217,11 @@
       <c r="D2398">
         <v>3</v>
       </c>
-    </row>
-    <row r="2399" spans="1:4">
+      <c r="E2398">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:8">
       <c r="A2399" s="1">
         <v>2397</v>
       </c>
@@ -51766,8 +52234,11 @@
       <c r="D2399">
         <v>1</v>
       </c>
-    </row>
-    <row r="2400" spans="1:4" ht="28.9">
+      <c r="E2399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:8" ht="28.9">
       <c r="A2400" s="1">
         <v>2398</v>
       </c>
@@ -51780,8 +52251,11 @@
       <c r="D2400">
         <v>1</v>
       </c>
-    </row>
-    <row r="2401" spans="1:4" ht="72">
+      <c r="E2400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:8" ht="72">
       <c r="A2401" s="1">
         <v>2399</v>
       </c>
@@ -51794,8 +52268,11 @@
       <c r="D2401">
         <v>2</v>
       </c>
-    </row>
-    <row r="2402" spans="1:4" ht="28.9">
+      <c r="F2401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:8" ht="28.9">
       <c r="A2402" s="1">
         <v>2400</v>
       </c>
@@ -51808,8 +52285,14 @@
       <c r="D2402">
         <v>2</v>
       </c>
-    </row>
-    <row r="2403" spans="1:4">
+      <c r="E2402">
+        <v>0</v>
+      </c>
+      <c r="F2402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:8">
       <c r="A2403" s="1">
         <v>2401</v>
       </c>
@@ -51822,8 +52305,11 @@
       <c r="D2403">
         <v>3</v>
       </c>
-    </row>
-    <row r="2404" spans="1:4" ht="100.9">
+      <c r="G2403">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:8" ht="100.9">
       <c r="A2404" s="1">
         <v>2402</v>
       </c>
@@ -51836,8 +52322,11 @@
       <c r="D2404">
         <v>3</v>
       </c>
-    </row>
-    <row r="2405" spans="1:4">
+      <c r="H2404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:8">
       <c r="A2405" s="1">
         <v>2403</v>
       </c>
@@ -51850,8 +52339,11 @@
       <c r="D2405">
         <v>3</v>
       </c>
-    </row>
-    <row r="2406" spans="1:4" ht="100.9">
+      <c r="E2405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:8" ht="100.9">
       <c r="A2406" s="1">
         <v>2404</v>
       </c>
@@ -51864,8 +52356,11 @@
       <c r="D2406">
         <v>3</v>
       </c>
-    </row>
-    <row r="2407" spans="1:4">
+      <c r="E2406">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:8">
       <c r="A2407" s="1">
         <v>2405</v>
       </c>
@@ -51878,8 +52373,11 @@
       <c r="D2407">
         <v>3</v>
       </c>
-    </row>
-    <row r="2408" spans="1:4" ht="43.15">
+      <c r="E2407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:8" ht="43.15">
       <c r="A2408" s="1">
         <v>2406</v>
       </c>
@@ -51892,8 +52390,11 @@
       <c r="D2408">
         <v>3</v>
       </c>
-    </row>
-    <row r="2409" spans="1:4" ht="28.9">
+      <c r="E2408">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:8" ht="28.9">
       <c r="A2409" s="1">
         <v>2407</v>
       </c>
@@ -51906,8 +52407,11 @@
       <c r="D2409">
         <v>1</v>
       </c>
-    </row>
-    <row r="2410" spans="1:4">
+      <c r="E2409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:8">
       <c r="A2410" s="1">
         <v>2408</v>
       </c>
@@ -51920,8 +52424,14 @@
       <c r="D2410">
         <v>3</v>
       </c>
-    </row>
-    <row r="2411" spans="1:4">
+      <c r="E2410">
+        <v>0</v>
+      </c>
+      <c r="H2410">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:8">
       <c r="A2411" s="1">
         <v>2409</v>
       </c>
@@ -51934,8 +52444,11 @@
       <c r="D2411">
         <v>1</v>
       </c>
-    </row>
-    <row r="2412" spans="1:4">
+      <c r="E2411">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:8">
       <c r="A2412" s="1">
         <v>2410</v>
       </c>
@@ -51948,8 +52461,11 @@
       <c r="D2412">
         <v>1</v>
       </c>
-    </row>
-    <row r="2413" spans="1:4" ht="28.9">
+      <c r="F2412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:8" ht="28.9">
       <c r="A2413" s="1">
         <v>2411</v>
       </c>
@@ -51962,8 +52478,11 @@
       <c r="D2413">
         <v>2</v>
       </c>
-    </row>
-    <row r="2414" spans="1:4" ht="28.9">
+      <c r="E2413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:8" ht="28.9">
       <c r="A2414" s="1">
         <v>2412</v>
       </c>
@@ -51976,8 +52495,11 @@
       <c r="D2414">
         <v>1</v>
       </c>
-    </row>
-    <row r="2415" spans="1:4">
+      <c r="E2414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:8">
       <c r="A2415" s="1">
         <v>2413</v>
       </c>
@@ -51990,8 +52512,11 @@
       <c r="D2415">
         <v>2</v>
       </c>
-    </row>
-    <row r="2416" spans="1:4">
+      <c r="E2415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:8">
       <c r="A2416" s="1">
         <v>2414</v>
       </c>
@@ -52004,8 +52529,11 @@
       <c r="D2416">
         <v>1</v>
       </c>
-    </row>
-    <row r="2417" spans="1:4">
+      <c r="E2416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:8">
       <c r="A2417" s="1">
         <v>2415</v>
       </c>
@@ -52018,8 +52546,11 @@
       <c r="D2417">
         <v>1</v>
       </c>
-    </row>
-    <row r="2418" spans="1:4" ht="28.9">
+      <c r="E2417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:8" ht="28.9">
       <c r="A2418" s="1">
         <v>2416</v>
       </c>
@@ -52032,8 +52563,14 @@
       <c r="D2418">
         <v>1</v>
       </c>
-    </row>
-    <row r="2419" spans="1:4">
+      <c r="E2418">
+        <v>0</v>
+      </c>
+      <c r="H2418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:8">
       <c r="A2419" s="1">
         <v>2417</v>
       </c>
@@ -52046,8 +52583,11 @@
       <c r="D2419">
         <v>1</v>
       </c>
-    </row>
-    <row r="2420" spans="1:4">
+      <c r="E2419">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:8">
       <c r="A2420" s="1">
         <v>2418</v>
       </c>
@@ -52060,8 +52600,11 @@
       <c r="D2420">
         <v>1</v>
       </c>
-    </row>
-    <row r="2421" spans="1:4">
+      <c r="E2420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:8">
       <c r="A2421" s="1">
         <v>2419</v>
       </c>
@@ -52074,8 +52617,14 @@
       <c r="D2421">
         <v>1</v>
       </c>
-    </row>
-    <row r="2422" spans="1:4">
+      <c r="E2421">
+        <v>0</v>
+      </c>
+      <c r="F2421">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:8">
       <c r="A2422" s="1">
         <v>2420</v>
       </c>
@@ -52088,8 +52637,11 @@
       <c r="D2422">
         <v>3</v>
       </c>
-    </row>
-    <row r="2423" spans="1:4" ht="43.15">
+      <c r="H2422">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:8" ht="43.15">
       <c r="A2423" s="1">
         <v>2421</v>
       </c>
@@ -52102,8 +52654,11 @@
       <c r="D2423">
         <v>2</v>
       </c>
-    </row>
-    <row r="2424" spans="1:4" ht="28.9">
+      <c r="E2423">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:8" ht="28.9">
       <c r="A2424" s="1">
         <v>2422</v>
       </c>
@@ -52116,8 +52671,11 @@
       <c r="D2424">
         <v>1</v>
       </c>
-    </row>
-    <row r="2425" spans="1:4" ht="230.45">
+      <c r="E2424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:8" ht="230.45">
       <c r="A2425" s="1">
         <v>2423</v>
       </c>
@@ -52130,8 +52688,14 @@
       <c r="D2425">
         <v>1</v>
       </c>
-    </row>
-    <row r="2426" spans="1:4" ht="43.15">
+      <c r="E2425">
+        <v>0</v>
+      </c>
+      <c r="F2425">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:8" ht="43.15">
       <c r="A2426" s="1">
         <v>2424</v>
       </c>
@@ -52144,8 +52708,14 @@
       <c r="D2426">
         <v>2</v>
       </c>
-    </row>
-    <row r="2427" spans="1:4">
+      <c r="E2426">
+        <v>0</v>
+      </c>
+      <c r="F2426">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:8">
       <c r="A2427" s="1">
         <v>2425</v>
       </c>
@@ -52158,8 +52728,11 @@
       <c r="D2427">
         <v>3</v>
       </c>
-    </row>
-    <row r="2428" spans="1:4">
+      <c r="E2427">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:8">
       <c r="A2428" s="1">
         <v>2426</v>
       </c>
@@ -52172,8 +52745,11 @@
       <c r="D2428">
         <v>2</v>
       </c>
-    </row>
-    <row r="2429" spans="1:4">
+      <c r="F2428">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:8">
       <c r="A2429" s="1">
         <v>2427</v>
       </c>
@@ -52186,8 +52762,11 @@
       <c r="D2429">
         <v>1</v>
       </c>
-    </row>
-    <row r="2430" spans="1:4">
+      <c r="E2429">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:8">
       <c r="A2430" s="1">
         <v>2428</v>
       </c>
@@ -52200,8 +52779,11 @@
       <c r="D2430">
         <v>1</v>
       </c>
-    </row>
-    <row r="2431" spans="1:4">
+      <c r="F2430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:8">
       <c r="A2431" s="1">
         <v>2429</v>
       </c>
@@ -52214,8 +52796,11 @@
       <c r="D2431">
         <v>1</v>
       </c>
-    </row>
-    <row r="2432" spans="1:4">
+      <c r="H2431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:8">
       <c r="A2432" s="1">
         <v>2430</v>
       </c>
@@ -52228,8 +52813,11 @@
       <c r="D2432">
         <v>1</v>
       </c>
-    </row>
-    <row r="2433" spans="1:4" ht="28.9">
+      <c r="E2432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:8" ht="28.9">
       <c r="A2433" s="1">
         <v>2431</v>
       </c>
@@ -52242,8 +52830,11 @@
       <c r="D2433">
         <v>2</v>
       </c>
-    </row>
-    <row r="2434" spans="1:4">
+      <c r="E2433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:8">
       <c r="A2434" s="1">
         <v>2432</v>
       </c>
@@ -52256,8 +52847,11 @@
       <c r="D2434">
         <v>1</v>
       </c>
-    </row>
-    <row r="2435" spans="1:4">
+      <c r="E2434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:8">
       <c r="A2435" s="1">
         <v>2433</v>
       </c>
@@ -52270,8 +52864,11 @@
       <c r="D2435">
         <v>1</v>
       </c>
-    </row>
-    <row r="2436" spans="1:4" ht="57.6">
+      <c r="G2435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:8" ht="57.6">
       <c r="A2436" s="1">
         <v>2434</v>
       </c>
@@ -52284,8 +52881,17 @@
       <c r="D2436">
         <v>3</v>
       </c>
-    </row>
-    <row r="2437" spans="1:4">
+      <c r="E2436">
+        <v>0</v>
+      </c>
+      <c r="G2436">
+        <v>0</v>
+      </c>
+      <c r="H2436">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:8">
       <c r="A2437" s="1">
         <v>2435</v>
       </c>
@@ -52298,8 +52904,14 @@
       <c r="D2437">
         <v>3</v>
       </c>
-    </row>
-    <row r="2438" spans="1:4" ht="115.15">
+      <c r="E2437">
+        <v>0</v>
+      </c>
+      <c r="H2437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:8" ht="115.15">
       <c r="A2438" s="1">
         <v>2436</v>
       </c>
@@ -52312,8 +52924,14 @@
       <c r="D2438">
         <v>1</v>
       </c>
-    </row>
-    <row r="2439" spans="1:4" ht="43.15">
+      <c r="E2438">
+        <v>0</v>
+      </c>
+      <c r="F2438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:8" ht="43.15">
       <c r="A2439" s="1">
         <v>2437</v>
       </c>
@@ -52326,8 +52944,11 @@
       <c r="D2439">
         <v>2</v>
       </c>
-    </row>
-    <row r="2440" spans="1:4" ht="28.9">
+      <c r="F2439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:8" ht="28.9">
       <c r="A2440" s="1">
         <v>2438</v>
       </c>
@@ -52340,8 +52961,11 @@
       <c r="D2440">
         <v>1</v>
       </c>
-    </row>
-    <row r="2441" spans="1:4">
+      <c r="E2440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:8">
       <c r="A2441" s="1">
         <v>2439</v>
       </c>
@@ -52354,8 +52978,11 @@
       <c r="D2441">
         <v>2</v>
       </c>
-    </row>
-    <row r="2442" spans="1:4">
+      <c r="E2441">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:8">
       <c r="A2442" s="1">
         <v>2440</v>
       </c>
@@ -52368,8 +52995,14 @@
       <c r="D2442">
         <v>3</v>
       </c>
-    </row>
-    <row r="2443" spans="1:4" ht="28.9">
+      <c r="E2442">
+        <v>0</v>
+      </c>
+      <c r="G2442">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:8" ht="28.9">
       <c r="A2443" s="1">
         <v>2441</v>
       </c>
@@ -52382,8 +53015,11 @@
       <c r="D2443">
         <v>1</v>
       </c>
-    </row>
-    <row r="2444" spans="1:4" ht="28.9">
+      <c r="E2443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:8" ht="28.9">
       <c r="A2444" s="1">
         <v>2442</v>
       </c>
@@ -52396,8 +53032,14 @@
       <c r="D2444">
         <v>1</v>
       </c>
-    </row>
-    <row r="2445" spans="1:4">
+      <c r="E2444">
+        <v>0</v>
+      </c>
+      <c r="F2444">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:8">
       <c r="A2445" s="1">
         <v>2443</v>
       </c>
@@ -52410,8 +53052,11 @@
       <c r="D2445">
         <v>3</v>
       </c>
-    </row>
-    <row r="2446" spans="1:4" ht="28.9">
+      <c r="H2445">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:8" ht="28.9">
       <c r="A2446" s="1">
         <v>2444</v>
       </c>
@@ -52424,8 +53069,14 @@
       <c r="D2446">
         <v>3</v>
       </c>
-    </row>
-    <row r="2447" spans="1:4" ht="28.9">
+      <c r="G2446">
+        <v>1</v>
+      </c>
+      <c r="H2446">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:8" ht="28.9">
       <c r="A2447" s="1">
         <v>2445</v>
       </c>
@@ -52438,8 +53089,11 @@
       <c r="D2447">
         <v>1</v>
       </c>
-    </row>
-    <row r="2448" spans="1:4">
+      <c r="F2447">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:8">
       <c r="A2448" s="1">
         <v>2446</v>
       </c>
@@ -52452,8 +53106,11 @@
       <c r="D2448">
         <v>2</v>
       </c>
-    </row>
-    <row r="2449" spans="1:4" ht="43.15">
+      <c r="E2448">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:7" ht="43.15">
       <c r="A2449" s="1">
         <v>2447</v>
       </c>
@@ -52466,8 +53123,11 @@
       <c r="D2449">
         <v>2</v>
       </c>
-    </row>
-    <row r="2450" spans="1:4">
+      <c r="F2449">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:7">
       <c r="A2450" s="1">
         <v>2448</v>
       </c>
@@ -52480,8 +53140,11 @@
       <c r="D2450">
         <v>1</v>
       </c>
-    </row>
-    <row r="2451" spans="1:4" ht="28.9">
+      <c r="E2450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:7" ht="28.9">
       <c r="A2451" s="1">
         <v>2449</v>
       </c>
@@ -52494,8 +53157,14 @@
       <c r="D2451">
         <v>1</v>
       </c>
-    </row>
-    <row r="2452" spans="1:4" ht="57.6">
+      <c r="E2451">
+        <v>0</v>
+      </c>
+      <c r="F2451">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:7" ht="57.6">
       <c r="A2452" s="1">
         <v>2450</v>
       </c>
@@ -52508,8 +53177,14 @@
       <c r="D2452">
         <v>2</v>
       </c>
-    </row>
-    <row r="2453" spans="1:4">
+      <c r="E2452">
+        <v>0</v>
+      </c>
+      <c r="F2452">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:7">
       <c r="A2453" s="1">
         <v>2451</v>
       </c>
@@ -52522,8 +53197,11 @@
       <c r="D2453">
         <v>2</v>
       </c>
-    </row>
-    <row r="2454" spans="1:4" ht="43.15">
+      <c r="E2453">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:7" ht="43.15">
       <c r="A2454" s="1">
         <v>2452</v>
       </c>
@@ -52536,8 +53214,14 @@
       <c r="D2454">
         <v>1</v>
       </c>
-    </row>
-    <row r="2455" spans="1:4" ht="43.15">
+      <c r="E2454">
+        <v>0</v>
+      </c>
+      <c r="F2454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:7" ht="43.15">
       <c r="A2455" s="1">
         <v>2453</v>
       </c>
@@ -52550,8 +53234,14 @@
       <c r="D2455">
         <v>2</v>
       </c>
-    </row>
-    <row r="2456" spans="1:4" ht="28.9">
+      <c r="E2455">
+        <v>0</v>
+      </c>
+      <c r="G2455">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:7" ht="28.9">
       <c r="A2456" s="1">
         <v>2454</v>
       </c>
@@ -52564,8 +53254,11 @@
       <c r="D2456">
         <v>1</v>
       </c>
-    </row>
-    <row r="2457" spans="1:4" ht="72">
+      <c r="E2456">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:7" ht="72">
       <c r="A2457" s="1">
         <v>2455</v>
       </c>
@@ -52578,8 +53271,11 @@
       <c r="D2457">
         <v>1</v>
       </c>
-    </row>
-    <row r="2458" spans="1:4" ht="86.45">
+      <c r="E2457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:7" ht="86.45">
       <c r="A2458" s="1">
         <v>2456</v>
       </c>
@@ -52592,8 +53288,17 @@
       <c r="D2458">
         <v>2</v>
       </c>
-    </row>
-    <row r="2459" spans="1:4">
+      <c r="E2458">
+        <v>0</v>
+      </c>
+      <c r="F2458">
+        <v>0</v>
+      </c>
+      <c r="G2458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:7">
       <c r="A2459" s="1">
         <v>2457</v>
       </c>
@@ -52606,8 +53311,11 @@
       <c r="D2459">
         <v>2</v>
       </c>
-    </row>
-    <row r="2460" spans="1:4" ht="28.9">
+      <c r="E2459">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:7" ht="28.9">
       <c r="A2460" s="1">
         <v>2458</v>
       </c>
@@ -52620,8 +53328,11 @@
       <c r="D2460">
         <v>1</v>
       </c>
-    </row>
-    <row r="2461" spans="1:4">
+      <c r="E2460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:7">
       <c r="A2461" s="1">
         <v>2459</v>
       </c>
@@ -52634,8 +53345,14 @@
       <c r="D2461">
         <v>2</v>
       </c>
-    </row>
-    <row r="2462" spans="1:4">
+      <c r="E2461">
+        <v>0</v>
+      </c>
+      <c r="F2461">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:7">
       <c r="A2462" s="1">
         <v>2460</v>
       </c>
@@ -52648,8 +53365,11 @@
       <c r="D2462">
         <v>1</v>
       </c>
-    </row>
-    <row r="2463" spans="1:4">
+      <c r="E2462">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:7">
       <c r="A2463" s="1">
         <v>2461</v>
       </c>
@@ -52662,8 +53382,11 @@
       <c r="D2463">
         <v>1</v>
       </c>
-    </row>
-    <row r="2464" spans="1:4">
+      <c r="E2463">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:7">
       <c r="A2464" s="1">
         <v>2462</v>
       </c>
@@ -52676,8 +53399,11 @@
       <c r="D2464">
         <v>3</v>
       </c>
-    </row>
-    <row r="2465" spans="1:4">
+      <c r="E2464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:8">
       <c r="A2465" s="1">
         <v>2463</v>
       </c>
@@ -52690,8 +53416,14 @@
       <c r="D2465">
         <v>3</v>
       </c>
-    </row>
-    <row r="2466" spans="1:4">
+      <c r="E2465">
+        <v>0</v>
+      </c>
+      <c r="H2465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:8">
       <c r="A2466" s="1">
         <v>2464</v>
       </c>
@@ -52704,8 +53436,11 @@
       <c r="D2466">
         <v>3</v>
       </c>
-    </row>
-    <row r="2467" spans="1:4" ht="43.15">
+      <c r="E2466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:8" ht="43.15">
       <c r="A2467" s="1">
         <v>2465</v>
       </c>
@@ -52718,8 +53453,14 @@
       <c r="D2467">
         <v>2</v>
       </c>
-    </row>
-    <row r="2468" spans="1:4">
+      <c r="F2467">
+        <v>0</v>
+      </c>
+      <c r="G2467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2468" spans="1:8">
       <c r="A2468" s="1">
         <v>2466</v>
       </c>
@@ -52732,8 +53473,14 @@
       <c r="D2468">
         <v>1</v>
       </c>
-    </row>
-    <row r="2469" spans="1:4">
+      <c r="E2468">
+        <v>1</v>
+      </c>
+      <c r="G2468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:8">
       <c r="A2469" s="1">
         <v>2467</v>
       </c>
@@ -52746,8 +53493,11 @@
       <c r="D2469">
         <v>3</v>
       </c>
-    </row>
-    <row r="2470" spans="1:4" ht="28.9">
+      <c r="E2469">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:8" ht="28.9">
       <c r="A2470" s="1">
         <v>2468</v>
       </c>
@@ -52760,8 +53510,11 @@
       <c r="D2470">
         <v>1</v>
       </c>
-    </row>
-    <row r="2471" spans="1:4" ht="43.15">
+      <c r="E2470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:8" ht="43.15">
       <c r="A2471" s="1">
         <v>2469</v>
       </c>
@@ -52774,8 +53527,14 @@
       <c r="D2471">
         <v>2</v>
       </c>
-    </row>
-    <row r="2472" spans="1:4" ht="28.9">
+      <c r="G2471">
+        <v>1</v>
+      </c>
+      <c r="H2471">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:8" ht="28.9">
       <c r="A2472" s="1">
         <v>2470</v>
       </c>
@@ -52788,8 +53547,11 @@
       <c r="D2472">
         <v>1</v>
       </c>
-    </row>
-    <row r="2473" spans="1:4" ht="28.9">
+      <c r="F2472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:8" ht="28.9">
       <c r="A2473" s="1">
         <v>2471</v>
       </c>
@@ -52802,8 +53564,11 @@
       <c r="D2473">
         <v>3</v>
       </c>
-    </row>
-    <row r="2474" spans="1:4">
+      <c r="E2473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:8">
       <c r="A2474" s="1">
         <v>2472</v>
       </c>
@@ -52816,8 +53581,11 @@
       <c r="D2474">
         <v>1</v>
       </c>
-    </row>
-    <row r="2475" spans="1:4">
+      <c r="E2474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:8">
       <c r="A2475" s="1">
         <v>2473</v>
       </c>
@@ -52830,8 +53598,11 @@
       <c r="D2475">
         <v>3</v>
       </c>
-    </row>
-    <row r="2476" spans="1:4" ht="72">
+      <c r="E2475">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:8" ht="72">
       <c r="A2476" s="1">
         <v>2474</v>
       </c>
@@ -52844,8 +53615,14 @@
       <c r="D2476">
         <v>2</v>
       </c>
-    </row>
-    <row r="2477" spans="1:4" ht="28.9">
+      <c r="E2476">
+        <v>0</v>
+      </c>
+      <c r="F2476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:8" ht="28.9">
       <c r="A2477" s="1">
         <v>2475</v>
       </c>
@@ -52858,8 +53635,14 @@
       <c r="D2477">
         <v>1</v>
       </c>
-    </row>
-    <row r="2478" spans="1:4" ht="28.9">
+      <c r="E2477">
+        <v>0</v>
+      </c>
+      <c r="F2477">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:8" ht="28.9">
       <c r="A2478" s="1">
         <v>2476</v>
       </c>
@@ -52872,8 +53655,11 @@
       <c r="D2478">
         <v>1</v>
       </c>
-    </row>
-    <row r="2479" spans="1:4" ht="43.15">
+      <c r="F2478">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:8" ht="43.15">
       <c r="A2479" s="1">
         <v>2477</v>
       </c>
@@ -52886,8 +53672,17 @@
       <c r="D2479">
         <v>3</v>
       </c>
-    </row>
-    <row r="2480" spans="1:4" ht="28.9">
+      <c r="E2479">
+        <v>0</v>
+      </c>
+      <c r="F2479">
+        <v>0</v>
+      </c>
+      <c r="H2479">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:8" ht="28.9">
       <c r="A2480" s="1">
         <v>2478</v>
       </c>
@@ -52900,8 +53695,17 @@
       <c r="D2480">
         <v>2</v>
       </c>
-    </row>
-    <row r="2481" spans="1:4">
+      <c r="E2480">
+        <v>0</v>
+      </c>
+      <c r="F2480">
+        <v>-1</v>
+      </c>
+      <c r="H2480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:8">
       <c r="A2481" s="1">
         <v>2479</v>
       </c>
@@ -52914,8 +53718,11 @@
       <c r="D2481">
         <v>2</v>
       </c>
-    </row>
-    <row r="2482" spans="1:4">
+      <c r="E2481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:8">
       <c r="A2482" s="1">
         <v>2480</v>
       </c>
@@ -52928,8 +53735,11 @@
       <c r="D2482">
         <v>1</v>
       </c>
-    </row>
-    <row r="2483" spans="1:4">
+      <c r="F2482">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:8">
       <c r="A2483" s="1">
         <v>2481</v>
       </c>
@@ -52942,8 +53752,11 @@
       <c r="D2483">
         <v>2</v>
       </c>
-    </row>
-    <row r="2484" spans="1:4">
+      <c r="E2483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:8">
       <c r="A2484" s="1">
         <v>2482</v>
       </c>
@@ -52956,8 +53769,11 @@
       <c r="D2484">
         <v>1</v>
       </c>
-    </row>
-    <row r="2485" spans="1:4" ht="28.9">
+      <c r="E2484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:8" ht="28.9">
       <c r="A2485" s="1">
         <v>2483</v>
       </c>
@@ -52970,8 +53786,11 @@
       <c r="D2485">
         <v>2</v>
       </c>
-    </row>
-    <row r="2486" spans="1:4" ht="72">
+      <c r="E2485">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:8" ht="72">
       <c r="A2486" s="1">
         <v>2484</v>
       </c>
@@ -52984,8 +53803,11 @@
       <c r="D2486">
         <v>1</v>
       </c>
-    </row>
-    <row r="2487" spans="1:4">
+      <c r="E2486">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:8">
       <c r="A2487" s="1">
         <v>2485</v>
       </c>
@@ -52998,8 +53820,11 @@
       <c r="D2487">
         <v>2</v>
       </c>
-    </row>
-    <row r="2488" spans="1:4">
+      <c r="E2487">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:8">
       <c r="A2488" s="1">
         <v>2486</v>
       </c>
@@ -53012,8 +53837,11 @@
       <c r="D2488">
         <v>1</v>
       </c>
-    </row>
-    <row r="2489" spans="1:4" ht="43.15">
+      <c r="E2488">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:8" ht="43.15">
       <c r="A2489" s="1">
         <v>2487</v>
       </c>
@@ -53026,8 +53854,14 @@
       <c r="D2489">
         <v>3</v>
       </c>
-    </row>
-    <row r="2490" spans="1:4" ht="28.9">
+      <c r="E2489">
+        <v>0</v>
+      </c>
+      <c r="F2489">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:8" ht="28.9">
       <c r="A2490" s="1">
         <v>2488</v>
       </c>
@@ -53040,8 +53874,11 @@
       <c r="D2490">
         <v>2</v>
       </c>
-    </row>
-    <row r="2491" spans="1:4">
+      <c r="E2490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:8">
       <c r="A2491" s="1">
         <v>2489</v>
       </c>
@@ -53054,8 +53891,11 @@
       <c r="D2491">
         <v>1</v>
       </c>
-    </row>
-    <row r="2492" spans="1:4" ht="57.6">
+      <c r="E2491">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:8" ht="57.6">
       <c r="A2492" s="1">
         <v>2490</v>
       </c>
@@ -53068,8 +53908,17 @@
       <c r="D2492">
         <v>3</v>
       </c>
-    </row>
-    <row r="2493" spans="1:4">
+      <c r="E2492">
+        <v>0</v>
+      </c>
+      <c r="G2492">
+        <v>1</v>
+      </c>
+      <c r="H2492">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2493" spans="1:8">
       <c r="A2493" s="1">
         <v>2491</v>
       </c>
@@ -53082,8 +53931,11 @@
       <c r="D2493">
         <v>2</v>
       </c>
-    </row>
-    <row r="2494" spans="1:4">
+      <c r="F2493">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:8">
       <c r="A2494" s="1">
         <v>2492</v>
       </c>
@@ -53096,8 +53948,11 @@
       <c r="D2494">
         <v>2</v>
       </c>
-    </row>
-    <row r="2495" spans="1:4">
+      <c r="F2494">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:8">
       <c r="A2495" s="1">
         <v>2493</v>
       </c>
@@ -53110,8 +53965,14 @@
       <c r="D2495">
         <v>1</v>
       </c>
-    </row>
-    <row r="2496" spans="1:4" ht="100.9">
+      <c r="E2495">
+        <v>0</v>
+      </c>
+      <c r="F2495">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:8" ht="100.9">
       <c r="A2496" s="1">
         <v>2494</v>
       </c>
@@ -53124,8 +53985,11 @@
       <c r="D2496">
         <v>1</v>
       </c>
-    </row>
-    <row r="2497" spans="1:4">
+      <c r="F2496">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:8">
       <c r="A2497" s="1">
         <v>2495</v>
       </c>
@@ -53138,8 +54002,11 @@
       <c r="D2497">
         <v>2</v>
       </c>
-    </row>
-    <row r="2498" spans="1:4">
+      <c r="E2497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:8">
       <c r="A2498" s="1">
         <v>2496</v>
       </c>
@@ -53152,8 +54019,11 @@
       <c r="D2498">
         <v>2</v>
       </c>
-    </row>
-    <row r="2499" spans="1:4" ht="43.15">
+      <c r="E2498">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:8" ht="43.15">
       <c r="A2499" s="1">
         <v>2497</v>
       </c>
@@ -53166,8 +54036,20 @@
       <c r="D2499">
         <v>2</v>
       </c>
-    </row>
-    <row r="2500" spans="1:4" ht="172.9">
+      <c r="E2499">
+        <v>0</v>
+      </c>
+      <c r="F2499">
+        <v>-1</v>
+      </c>
+      <c r="G2499">
+        <v>1</v>
+      </c>
+      <c r="H2499">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:8" ht="172.9">
       <c r="A2500" s="1">
         <v>2498</v>
       </c>
@@ -53180,8 +54062,11 @@
       <c r="D2500">
         <v>1</v>
       </c>
-    </row>
-    <row r="2501" spans="1:4">
+      <c r="E2500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:8">
       <c r="A2501" s="1">
         <v>2499</v>
       </c>
@@ -53193,6 +54078,9 @@
       </c>
       <c r="D2501">
         <v>1</v>
+      </c>
+      <c r="E2501">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>